<commit_message>
fix but i don't know why
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B66"/>
+  <dimension ref="A2:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,780 +424,432 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AXSM-EC-SOL</t>
+          <t>PP-AI3-LCD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>57,50</t>
+          <t>18,93</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IPXSM-HOLED</t>
+          <t>A1389-BAT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>36,50</t>
+          <t>17,01</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IPXS-CARR</t>
+          <t>PP-AI4-TCB+</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>25,70</t>
+          <t>5,51</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>116633</t>
+          <t>PP-AI4-TCN+</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>23,70</t>
+          <t>5,23</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IPXSM-EC-INC</t>
+          <t>A1416-CARR</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>21,50</t>
+          <t>1,62</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>123275</t>
+          <t>PP-AI3-WIFI</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14,20</t>
+          <t>1,43</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A1921-BAT-TI</t>
+          <t>A1416-CAVT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9,03</t>
+          <t>1,33</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>513339</t>
+          <t>PP-AI4-CC</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7,51</t>
+          <t>1,31</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IPXSMBAT-WBMS</t>
+          <t>PP-AI4-VOL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7,13</t>
+          <t>0,98</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IPXSM-CCB-REL</t>
+          <t>PP-AI4-NBH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7,20</t>
+          <t>0,86</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PP0290</t>
+          <t>PP-AI3-CHAN</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6,56</t>
+          <t>0,86</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IPXSM-CCO-REL</t>
+          <t>PP-AI3-CHAB</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6,60</t>
+          <t>0,48</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IPXSM-CCN-REL</t>
+          <t>PP-AI3-LCD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>6,00</t>
+          <t>18,93</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>462876</t>
+          <t>A1389-BAT</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5,46</t>
+          <t>17,01</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IXS-U_WLAN_W</t>
+          <t>PP-AI4-TCB+</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4,18</t>
+          <t>5,51</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>142689</t>
+          <t>PP-AI4-TCN+</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3,71</t>
+          <t>5,23</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AXSM-QIVOL</t>
+          <t>A1416-CARR</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3,42</t>
+          <t>1,62</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AXSM-PROX</t>
+          <t>PP-AI3-WIFI</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3,33</t>
+          <t>1,43</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AXSM-LECTSIM</t>
+          <t>A1416-CAVT</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3,04</t>
+          <t>1,33</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AXSM-VOL</t>
+          <t>PP-AI4-CC</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2,71</t>
+          <t>1,31</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AXSM-WIFI</t>
+          <t>PP-AI4-VOL</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2,09</t>
+          <t>0,98</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IXSM-CAMAV-IR</t>
+          <t>PP-AI4-NBH</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1,71</t>
+          <t>0,86</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>IPXSM-VAN-LH</t>
+          <t>PP-AI3-CHAN</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1,62</t>
+          <t>0,86</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>I8-U6300</t>
+          <t>PP-AI3-CHAB</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1,62</t>
+          <t>0,48</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IX-U4700</t>
+          <t>PP-AI3-LCD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1,52</t>
+          <t>18,93</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IPXSM-VAB-LH</t>
+          <t>A1389-BAT</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1,43</t>
+          <t>17,01</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IX-U4400</t>
+          <t>PP-AI4-TCB+</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1,31</t>
+          <t>5,51</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>IPXS-LENC</t>
+          <t>PP-AI4-TCN+</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1,24</t>
+          <t>5,23</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AXSM-VIB</t>
+          <t>A1416-CARR</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1,24</t>
+          <t>1,62</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PP5314</t>
+          <t>PP-AI3-WIFI</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1,14</t>
+          <t>1,43</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AXS-GPS</t>
+          <t>A1416-CAVT</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1,14</t>
+          <t>1,33</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>IXS-338S00425</t>
+          <t>PP-AI4-CC</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1,05</t>
+          <t>1,31</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AXS-POW</t>
+          <t>PP-AI4-VOL</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1,05</t>
+          <t>0,98</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>IX-U5600</t>
+          <t>PP-AI4-NBH</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1,01</t>
+          <t>0,86</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>I8-U3400</t>
+          <t>PP-AI3-CHAN</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0,92</t>
+          <t>0,86</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>IXS-J5800</t>
+          <t>PP-AI3-CHAB</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>IXS-JLAT_A</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>IXS-J3500</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>IXS-J3900</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>IXS-J4600</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>IXS-338S00411</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>IXS-U3300</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>0,86</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>IXS-J_UAT2</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>0,85</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>IXS-J_UAT1</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>0,85</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>IXS-J4300</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>0,76</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>IXS-J4500</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>0,76</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>IXS-J6400</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>0,76</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>IXS-J4000</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>0,76</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>IX-U4210</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>0,70</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>I8-J3200</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>0,67</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>AXSM-SBAT</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>AXSM-SIMO</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>0,49</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>AXSM-SIMA</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>0,49</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>AXSM-SIMGS</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>0,49</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>526979</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>0,50</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>IXS-CCSOUD-N</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>0,50</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>IXS-CCSOUD-O</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>0,50</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>IXS-J5400</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
           <t>0,48</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>IXS-J5700</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>0,48</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>PP5313</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>0,48</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>AXMS-BUZZ</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>0,48</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>IPXSM-VAO-LH</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>IPXSM-ADHBMS</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>1,26</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>IX-U3100</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>1,14</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>AXSM-ADHEN</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>0,40</t>
         </is>
       </c>
     </row>

</xml_diff>